<commit_message>
MS: vyplneni a kontrola dalsiho formulare
</commit_message>
<xml_diff>
--- a/src/main/java/webtest/work/dataSet/Default.xlsx
+++ b/src/main/java/webtest/work/dataSet/Default.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360" xr2:uid="{2CF69960-4841-48BE-BC7D-FAAEC6859BBA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360" activeTab="1" xr2:uid="{2CF69960-4841-48BE-BC7D-FAAEC6859BBA}"/>
   </bookViews>
   <sheets>
     <sheet name="NewPerson1" sheetId="1" r:id="rId1"/>
+    <sheet name="CZ_HPP" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>Jméno</t>
   </si>
@@ -66,6 +67,39 @@
   </si>
   <si>
     <t>01.10.2018</t>
+  </si>
+  <si>
+    <t>Titul</t>
+  </si>
+  <si>
+    <t>Rodné číslo</t>
+  </si>
+  <si>
+    <t>Číslo OP</t>
+  </si>
+  <si>
+    <t>Ulice</t>
+  </si>
+  <si>
+    <t>PSČ</t>
+  </si>
+  <si>
+    <t>Město</t>
+  </si>
+  <si>
+    <t>Ing.</t>
+  </si>
+  <si>
+    <t>Testerská 1234</t>
+  </si>
+  <si>
+    <t>Praha</t>
+  </si>
+  <si>
+    <t>001017/6573</t>
+  </si>
+  <si>
+    <t>222222222</t>
   </si>
 </sst>
 </file>
@@ -112,7 +146,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -130,10 +164,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutrální" xfId="1" builtinId="28"/>
@@ -451,8 +486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9C693CB-9CB2-4BF8-AC73-B742D86CDAF3}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,49 +500,49 @@
     <col min="7" max="7" width="38.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -518,4 +553,96 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="597" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56F79B08-CF7A-4884-A994-BC96F5DD2D02}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="1" t="str">
+        <f>NewPerson1!A2</f>
+        <v>Tester</v>
+      </c>
+      <c r="C2" s="1" t="str">
+        <f>NewPerson1!B2</f>
+        <v>Testerovič</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="1" t="str">
+        <f>NewPerson1!C2</f>
+        <v>tester.testerovic@email.com</v>
+      </c>
+      <c r="G2" s="1" t="str">
+        <f>NewPerson1!D2</f>
+        <v>+420 123 456 789</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2">
+        <v>33333</v>
+      </c>
+      <c r="J2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="597" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
MS: predelani par veci
</commit_message>
<xml_diff>
--- a/src/main/java/webtest/work/dataSet/Default.xlsx
+++ b/src/main/java/webtest/work/dataSet/Default.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\Desktop\ATM_selenium\ATM_selenium\src\main\java\webtest\work\dataSet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\péc\IdeaProjects\gitRepo\ATM_selenium\src\main\java\webtest\work\dataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="53">
   <si>
     <t>Jméno</t>
   </si>
@@ -115,6 +115,75 @@
   </si>
   <si>
     <t>Projektový manažer</t>
+  </si>
+  <si>
+    <t>Smlouva</t>
+  </si>
+  <si>
+    <t>HPP</t>
+  </si>
+  <si>
+    <t>Mzda</t>
+  </si>
+  <si>
+    <t>30000</t>
+  </si>
+  <si>
+    <t>Forma předání</t>
+  </si>
+  <si>
+    <t>Převodem na účet</t>
+  </si>
+  <si>
+    <t>Předčíslí</t>
+  </si>
+  <si>
+    <t>Číslo účtu</t>
+  </si>
+  <si>
+    <t>Kód banky</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>987654321</t>
+  </si>
+  <si>
+    <t>0300</t>
+  </si>
+  <si>
+    <t>Dovolená</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>Dovolená zbytek</t>
+  </si>
+  <si>
+    <t>Datum nástupu</t>
+  </si>
+  <si>
+    <t>Na dobu neurčitou</t>
+  </si>
+  <si>
+    <t>ANO</t>
+  </si>
+  <si>
+    <t>Zkušební doba</t>
+  </si>
+  <si>
+    <t>Počet dnů</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Stravenky</t>
+  </si>
+  <si>
+    <t>Výše úvazku</t>
   </si>
 </sst>
 </file>
@@ -179,11 +248,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutrální" xfId="1" builtinId="28"/>
@@ -505,17 +575,17 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -538,7 +608,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -572,25 +642,33 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56F79B08-CF7A-4884-A994-BC96F5DD2D02}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.6640625" customWidth="1"/>
-    <col min="12" max="12" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>14</v>
       </c>
@@ -627,8 +705,53 @@
       <c r="L1" s="3" t="s">
         <v>28</v>
       </c>
+      <c r="M1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -668,6 +791,53 @@
       </c>
       <c r="L2" t="s">
         <v>29</v>
+      </c>
+      <c r="M2" s="1" t="str">
+        <f>NewPerson1!E2</f>
+        <v>Ing. Jan Adminov</v>
+      </c>
+      <c r="N2" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P2" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="V2" s="1" t="str">
+        <f>NewPerson1!F2</f>
+        <v>01.10.2018</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA2" s="4">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MS: Step 3 checkovani a vyplnovani
</commit_message>
<xml_diff>
--- a/src/main/java/webtest/work/dataSet/Default.xlsx
+++ b/src/main/java/webtest/work/dataSet/Default.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="99">
   <si>
     <t>Jméno</t>
   </si>
@@ -174,9 +174,6 @@
     <t>Zkušební doba</t>
   </si>
   <si>
-    <t>Počet dnů</t>
-  </si>
-  <si>
     <t>3</t>
   </si>
   <si>
@@ -184,13 +181,154 @@
   </si>
   <si>
     <t>Výše úvazku</t>
+  </si>
+  <si>
+    <t>positionSelectStep3</t>
+  </si>
+  <si>
+    <t>managerSelectStep3</t>
+  </si>
+  <si>
+    <t>contractSelectStep3</t>
+  </si>
+  <si>
+    <t>formOfWageSelectStep3</t>
+  </si>
+  <si>
+    <t>undefinedTermSelectStep3</t>
+  </si>
+  <si>
+    <t>testTermSelectStep3</t>
+  </si>
+  <si>
+    <t>fteSelectStep3</t>
+  </si>
+  <si>
+    <t>Prosím vyberte pozici z číselníku</t>
+  </si>
+  <si>
+    <t>Test Analytik</t>
+  </si>
+  <si>
+    <t>Test Designer</t>
+  </si>
+  <si>
+    <t>Test Manažer</t>
+  </si>
+  <si>
+    <t>IT Analytik</t>
+  </si>
+  <si>
+    <t>Office manager</t>
+  </si>
+  <si>
+    <t>Managing partner</t>
+  </si>
+  <si>
+    <t>Interní HPP</t>
+  </si>
+  <si>
+    <t>Vývojář</t>
+  </si>
+  <si>
+    <t>Obchodní manažer</t>
+  </si>
+  <si>
+    <t>IT specialista</t>
+  </si>
+  <si>
+    <t>Forma předání mzdy - prosím vyberte</t>
+  </si>
+  <si>
+    <t>Osobně v hotovosti</t>
+  </si>
+  <si>
+    <t>Prosím vyberte</t>
+  </si>
+  <si>
+    <t>100% (40 hod./týden)</t>
+  </si>
+  <si>
+    <t>50% (20 hod./týden)</t>
+  </si>
+  <si>
+    <t>60% (24 hod./týden)</t>
+  </si>
+  <si>
+    <t>62,5% (25 hod./týden)</t>
+  </si>
+  <si>
+    <t>70% (28 hod./týden)</t>
+  </si>
+  <si>
+    <t>75% (30 hod./týden)</t>
+  </si>
+  <si>
+    <t>80% (32 hod./týden)</t>
+  </si>
+  <si>
+    <t>87,5% (35 hod./týden)</t>
+  </si>
+  <si>
+    <t>80% (36 hod./týden)</t>
+  </si>
+  <si>
+    <t>NE</t>
+  </si>
+  <si>
+    <t>ANO (napište počet měsíců)</t>
+  </si>
+  <si>
+    <t>text fields values</t>
+  </si>
+  <si>
+    <t>Prosím vyberte manažera z číselníku</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                  Ing. Jan Adminov</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                  Bc. Andrea Bílá</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                  Ing. Tonik brambora</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                  Ing. Tomáš Hlavní</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                   Tomáš Spící</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                   Šárka Usměvavá</t>
+  </si>
+  <si>
+    <t>Prosím vyberte smlouvu z číselníku</t>
+  </si>
+  <si>
+    <t>NE (vyplňte datum do)</t>
+  </si>
+  <si>
+    <t>Poznámka_1234567890/*-+</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>Poznámka</t>
+  </si>
+  <si>
+    <t>select fields values</t>
+  </si>
+  <si>
+    <t>Počet měsíců</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -215,8 +353,30 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -234,6 +394,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -248,12 +414,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutrální" xfId="1" builtinId="28"/>
@@ -642,33 +815,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56F79B08-CF7A-4884-A994-BC96F5DD2D02}">
-  <dimension ref="A1:AA2"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="AA2" sqref="AA2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="4"/>
+    <col min="3" max="3" width="10.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" style="4" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="4"/>
+    <col min="11" max="11" width="15.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="4"/>
+    <col min="15" max="15" width="17.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>14</v>
       </c>
@@ -703,141 +878,333 @@
         <v>25</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z1" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AA1" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="1" t="str">
+      <c r="B2" s="4" t="str">
         <f>NewPerson1!A2</f>
         <v>Tester</v>
       </c>
-      <c r="C2" s="1" t="str">
+      <c r="C2" s="4" t="str">
         <f>NewPerson1!B2</f>
         <v>Testerovič</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="1" t="str">
+      <c r="F2" s="4" t="str">
         <f>NewPerson1!C2</f>
         <v>tester.testerovic@email.com</v>
       </c>
-      <c r="G2" s="1" t="str">
+      <c r="G2" s="4" t="str">
         <f>NewPerson1!D2</f>
         <v>+420 123 456 789</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="M2" s="1" t="str">
+      <c r="G5" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="4" t="str">
         <f>NewPerson1!E2</f>
         <v>Ing. Jan Adminov</v>
       </c>
-      <c r="N2" t="s">
+      <c r="C24" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="O2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="P2" t="s">
+      <c r="D24" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="Q2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="V2" s="1" t="str">
-        <f>NewPerson1!F2</f>
-        <v>01.10.2018</v>
-      </c>
-      <c r="W2" s="1" t="s">
+      <c r="E24" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="F24" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="Y2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AA2" s="4">
-        <v>1</v>
+      <c r="G24" s="4" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MS: KROK 4 !!!
</commit_message>
<xml_diff>
--- a/src/main/java/webtest/work/dataSet/Default.xlsx
+++ b/src/main/java/webtest/work/dataSet/Default.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="97">
   <si>
     <t>Jméno</t>
   </si>
@@ -174,9 +174,6 @@
     <t>Zkušební doba</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
     <t>Stravenky</t>
   </si>
   <si>
@@ -319,9 +316,6 @@
   </si>
   <si>
     <t>select fields values</t>
-  </si>
-  <si>
-    <t>Počet měsíců</t>
   </si>
 </sst>
 </file>
@@ -818,7 +812,7 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,7 +872,7 @@
         <v>25</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -925,86 +919,86 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="E5" s="7" t="s">
         <v>61</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>62</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>29</v>
       </c>
       <c r="G5" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="H5" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="I5" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="J5" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="K5" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="L5" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="M5" s="7" t="s">
         <v>68</v>
-      </c>
-      <c r="M5" s="7" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="C7" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="D7" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="E7" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="F7" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="G7" s="7" t="s">
         <v>90</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>31</v>
@@ -1012,15 +1006,15 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>70</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>71</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>35</v>
@@ -1028,7 +1022,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -1036,65 +1030,65 @@
         <v>47</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="C17" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="D17" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="E17" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="F17" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="G17" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="G17" s="7" t="s">
+      <c r="H17" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="H17" s="7" t="s">
+      <c r="I17" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="I17" s="7" t="s">
+      <c r="J17" s="7" t="s">
         <v>80</v>
-      </c>
-      <c r="J17" s="7" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
@@ -1120,10 +1114,7 @@
         <v>45</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1149,15 +1140,12 @@
         <v>13</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="I21" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1180,16 +1168,15 @@
         <v>48</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="4" t="str">
-        <f>NewPerson1!E2</f>
-        <v>Ing. Jan Adminov</v>
+      <c r="B24" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>31</v>
@@ -1204,7 +1191,7 @@
         <v>47</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MS: step 4 done
</commit_message>
<xml_diff>
--- a/src/main/java/webtest/work/dataSet/Default.xlsx
+++ b/src/main/java/webtest/work/dataSet/Default.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\péc\IdeaProjects\gitRepo\ATM_selenium\src\main\java\webtest\work\dataSet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\Desktop\ATM_selenium\ATM_selenium\src\main\java\webtest\work\dataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="128">
   <si>
     <t>Jméno</t>
   </si>
@@ -316,6 +316,99 @@
   </si>
   <si>
     <t>select fields values</t>
+  </si>
+  <si>
+    <t>STEP 3:</t>
+  </si>
+  <si>
+    <t>STEP 4:</t>
+  </si>
+  <si>
+    <t>Bez licence</t>
+  </si>
+  <si>
+    <t>G-Suite standard</t>
+  </si>
+  <si>
+    <t>G-Suite + MS Office desktop</t>
+  </si>
+  <si>
+    <t>licenseSelectStep4</t>
+  </si>
+  <si>
+    <t>tariffSelectStep4</t>
+  </si>
+  <si>
+    <t>infoPortalSelectStep4</t>
+  </si>
+  <si>
+    <t>hrmSelectStep4</t>
+  </si>
+  <si>
+    <t>projectsSelectStep4</t>
+  </si>
+  <si>
+    <t>Bez telefonního tarifu</t>
+  </si>
+  <si>
+    <t>Tarif 1 (524 CZK vč. DPH, 2.5 Gb + neomezené volání)</t>
+  </si>
+  <si>
+    <t>Tarif 2 (699 CZK vč. DPH, 5.0 Gb + neomezené volání + roaming)</t>
+  </si>
+  <si>
+    <t>WORK InfoPortál - vyberte požadovanou roli</t>
+  </si>
+  <si>
+    <t>Zaměstnanec</t>
+  </si>
+  <si>
+    <t>Správce</t>
+  </si>
+  <si>
+    <t>WORK HRM - vyberte požadovanou roli</t>
+  </si>
+  <si>
+    <t>Team Leader</t>
+  </si>
+  <si>
+    <t>WORK Projekty - vyberte požadovanou roli</t>
+  </si>
+  <si>
+    <t>Běžný zaměstnanec</t>
+  </si>
+  <si>
+    <t>Test Team Leader</t>
+  </si>
+  <si>
+    <t>Projektový Manažer</t>
+  </si>
+  <si>
+    <t>Vedení společnosti - přehledy</t>
+  </si>
+  <si>
+    <t>Licence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tarif </t>
+  </si>
+  <si>
+    <t>Role InfoPortal</t>
+  </si>
+  <si>
+    <t>Role HRM</t>
+  </si>
+  <si>
+    <t>Role Projekty</t>
+  </si>
+  <si>
+    <t>G-Suite</t>
+  </si>
+  <si>
+    <t>TT_leader</t>
+  </si>
+  <si>
+    <t>Tarif 1 (524)</t>
   </si>
 </sst>
 </file>
@@ -370,7 +463,7 @@
       <charset val="238"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -390,7 +483,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -408,19 +513,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutrální" xfId="1" builtinId="28"/>
@@ -742,17 +848,17 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -775,7 +881,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -809,391 +915,545 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56F79B08-CF7A-4884-A994-BC96F5DD2D02}">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="4"/>
-    <col min="3" max="3" width="10.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11" style="4" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="4"/>
-    <col min="11" max="11" width="15.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="4"/>
-    <col min="15" max="15" width="17.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="22.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" style="3"/>
+    <col min="3" max="3" width="10.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="15.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" style="3" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" style="3"/>
+    <col min="11" max="11" width="15.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.109375" style="3"/>
+    <col min="15" max="15" width="17.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="9" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="4" t="str">
+      <c r="B2" s="3" t="str">
         <f>NewPerson1!A2</f>
         <v>Tester</v>
       </c>
-      <c r="C2" s="4" t="str">
+      <c r="C2" s="3" t="str">
         <f>NewPerson1!B2</f>
         <v>Testerovič</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="4" t="str">
+      <c r="F2" s="3" t="str">
         <f>NewPerson1!C2</f>
         <v>tester.testerovic@email.com</v>
       </c>
-      <c r="G2" s="4" t="str">
+      <c r="G2" s="3" t="str">
         <f>NewPerson1!D2</f>
         <v>+420 123 456 789</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="3" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="J5" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="K5" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="L5" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="M5" s="7" t="s">
+      <c r="M5" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="4" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="G17" s="7" t="s">
+      <c r="G17" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="H17" s="7" t="s">
+      <c r="H17" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="I17" s="7" t="s">
+      <c r="I17" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="J17" s="7" t="s">
+      <c r="J17" s="4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+    <row r="20" spans="1:10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="G20" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="H20" s="9" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="F21" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="G21" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H21" s="4" t="s">
+      <c r="H21" s="3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="E23" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="F23" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="G23" s="6" t="s">
+      <c r="G23" s="7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F24" s="7" t="s">
+      <c r="F24" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="G24" s="4" t="s">
+      <c r="G24" s="3" t="s">
         <v>94</v>
       </c>
     </row>
+    <row r="25" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" s="7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="597" r:id="rId1"/>

</xml_diff>